<commit_message>
added dependencies and classes
</commit_message>
<xml_diff>
--- a/documentation/Check.xlsx
+++ b/documentation/Check.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="34">
   <si>
     <t>№;</t>
   </si>
@@ -41,7 +41,16 @@
     <t>Pass</t>
   </si>
   <si>
+    <t>Иногда получается зайти только со второго раза с валидными данными, закономерности не выявила</t>
+  </si>
+  <si>
     <t>Да</t>
+  </si>
+  <si>
+    <t>Авторизация с невалидными данными не проходит</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
   <si>
     <t>Новости</t>
@@ -50,10 +59,10 @@
     <t>Можно создать новую новость</t>
   </si>
   <si>
-    <t>Иногда получается зайти только со второго раза с валидными данными, закономерности не выявила</t>
+    <t>Нет</t>
   </si>
   <si>
-    <t>Нет</t>
+    <t>Список новостей отображается</t>
   </si>
   <si>
     <t>Цитаты (бабочка)</t>
@@ -62,10 +71,22 @@
     <t>Отображается список цитат</t>
   </si>
   <si>
+    <t>Цитаты можно расщелкнуть и увидеть описание</t>
+  </si>
+  <si>
     <t>О приложении</t>
   </si>
   <si>
     <t>Есть ссылки на Политику конфиденциальности и Пользовательское соглашение</t>
+  </si>
+  <si>
+    <t>Ссылки на Политику конфиденциальности и Пользовательское соглашение открываются и отображается содержимое</t>
+  </si>
+  <si>
+    <t>Выход</t>
+  </si>
+  <si>
+    <t>Проверка выхода из системы (Logout)</t>
   </si>
   <si>
     <r>
@@ -85,9 +106,6 @@
   </si>
   <si>
     <t>Вход с пустыми полями</t>
-  </si>
-  <si>
-    <t>Fail</t>
   </si>
   <si>
     <t>Отображается список новостей</t>
@@ -443,29 +461,28 @@
       <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="6"/>
+      <c r="E2" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F2" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3">
         <v>2.0</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4">
@@ -473,16 +490,16 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>9</v>
+      <c r="F4" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5">
@@ -490,33 +507,125 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="C6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="E6" s="6"/>
+      <c r="F6" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="7">
-      <c r="E7" s="6"/>
+      <c r="A7" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="8">
+      <c r="A8" s="3">
+        <v>7.0</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="E8" s="6"/>
+      <c r="F8" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="9">
+      <c r="A9" s="3">
+        <v>8.0</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="E9" s="6"/>
-    </row>
-    <row r="11">
-      <c r="E11" s="6"/>
+      <c r="F9" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3">
+        <v>9.0</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
+      <c r="Z10" s="6"/>
     </row>
     <row r="12">
       <c r="E12" s="6"/>
@@ -4491,13 +4600,13 @@
         <v>7.0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2">
@@ -4505,13 +4614,13 @@
         <v>8.0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">
@@ -4519,19 +4628,19 @@
         <v>9.0</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4">
@@ -4539,13 +4648,13 @@
         <v>10.0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
@@ -4553,10 +4662,10 @@
         <v>11.0</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>8</v>
@@ -4567,10 +4676,10 @@
         <v>12.0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>8</v>
@@ -4581,10 +4690,10 @@
         <v>13.0</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>8</v>
@@ -4595,10 +4704,10 @@
         <v>14.0</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>8</v>
@@ -4609,7 +4718,7 @@
         <v>15.0</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C9" s="6"/>
     </row>

</xml_diff>